<commit_message>
added use cases and pre processing merch updates
</commit_message>
<xml_diff>
--- a/use_cases.xlsx
+++ b/use_cases.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nosta\CODING\ist_dash_2024_rec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Coding\Python\ist_dash_2024_rec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47F8619C-6522-4025-9F7F-B7AB6FF4A1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FD97EB-DE30-4AAA-BA41-AB74C454E5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F51D9638-9F0E-44DB-995D-95F1B04E212F}"/>
+    <workbookView xWindow="-38510" yWindow="-3770" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{F51D9638-9F0E-44DB-995D-95F1B04E212F}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="encoding" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>event time</t>
   </si>
@@ -82,6 +83,60 @@
   </si>
   <si>
     <t>purchase, atc, etc</t>
+  </si>
+  <si>
+    <t>hierarchy enconding</t>
+  </si>
+  <si>
+    <t>A-Z order?</t>
+  </si>
+  <si>
+    <t>cat1</t>
+  </si>
+  <si>
+    <t>cat2</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>cat encoded</t>
+  </si>
+  <si>
+    <t>cat 2 encoded</t>
+  </si>
+  <si>
+    <t>brand encoded</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>tv</t>
+  </si>
+  <si>
+    <t>lg</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>home appliances</t>
+  </si>
+  <si>
+    <t>fridge</t>
+  </si>
+  <si>
+    <t>whirlpool</t>
+  </si>
+  <si>
+    <t>apparell</t>
+  </si>
+  <si>
+    <t>tshirts</t>
+  </si>
+  <si>
+    <t>nike</t>
   </si>
 </sst>
 </file>
@@ -132,13 +187,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +215,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -455,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266EFF46-B9F2-4E07-BE80-EA4EC77C90D9}">
   <dimension ref="C4:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -505,52 +563,52 @@
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>123</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I11" t="s">
@@ -558,7 +616,7 @@
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H12">
@@ -614,4 +672,152 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047C104A-DD27-4276-8E4B-CCEFE83D4B19}">
+  <dimension ref="I11:N20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="270" zoomScaleNormal="270" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="9:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>